<commit_message>
Edited the BOM, cleaned up some errors.
</commit_message>
<xml_diff>
--- a/communications_hub/Teensy_CommBus_BOM.xlsx
+++ b/communications_hub/Teensy_CommBus_BOM.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ydot/Documents/eagle/ARVP/communications_hub/communication-hub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\au_hardware\communications_hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25596" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -56,27 +56,6 @@
     <t>Teensy+i2c+CAN part list</t>
   </si>
   <si>
-    <t>DIL VERTICAL PC TAIL PIN HEADER 2x3</t>
-  </si>
-  <si>
-    <t>M20-9980345</t>
-  </si>
-  <si>
-    <t>https://cdn.harwin.com/pdfs/M20-998.pdf</t>
-  </si>
-  <si>
-    <t>DIL VERTICAL PC TAIL PIN HEADER 2x4</t>
-  </si>
-  <si>
-    <t>M20-9980445</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
-    <t>RC1206FR-0710KL</t>
-  </si>
-  <si>
     <t>http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_7.pdf</t>
   </si>
   <si>
@@ -101,15 +80,6 @@
     <t>http://www.samsungsem.com/kr/support/product-search/mlcc/CL21B106KOQNNNG.jsp</t>
   </si>
   <si>
-    <t>CONN HEADER GH SIDE 3POS 1.25MM</t>
-  </si>
-  <si>
-    <t>SM03B-GHS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>http://www.jst-mfg.com/product/pdf/eng/eGH.pdf</t>
-  </si>
-  <si>
     <t>IC TXRX CAN FAULT PROT 8SOIC</t>
   </si>
   <si>
@@ -134,15 +104,6 @@
     <t>https://cdn.harwin.com/pdfs/M20-999.pdf</t>
   </si>
   <si>
-    <t>CONN HEADER FMALE 14POS .1" GOLD</t>
-  </si>
-  <si>
-    <t>PPPC141LFBN-RC</t>
-  </si>
-  <si>
-    <t>http://www.sullinscorp.com/drawings/78_P(N)PxCxxxLFBN-RC,_10492-H.pdf</t>
-  </si>
-  <si>
     <t>LED YELLOW CLEAR 1206 SMD</t>
   </si>
   <si>
@@ -191,9 +152,6 @@
     <t>SSQ-115-03-T-D</t>
   </si>
   <si>
-    <t>RES SMD 120 OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
     <t>CONN HEADER GH SIDE 4POS 1.25MM</t>
   </si>
   <si>
@@ -212,17 +170,26 @@
     <t>https://www.digikey.ca/product-detail/en/jst-sales-america-inc/SM02B-GHS-TB-LF-SN/455-1564-1-ND/807832</t>
   </si>
   <si>
-    <t>RC3216F121CS</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/samsung-electro-mechanics/RC3216F121CS/1276-5672-1-ND/3968644</t>
+  </si>
+  <si>
+    <t>RC0805FR-0710KL</t>
+  </si>
+  <si>
+    <t>RES SMD 62 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>311-62ERCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/8W 0805</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +209,12 @@
       <sz val="12"/>
       <color rgb="FF24292E"/>
       <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -292,18 +265,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -584,33 +558,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="63.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,426 +607,350 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="1">
-        <v>0.34799999999999998</v>
+        <v>4.7E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G10" si="0">F3*E3</f>
-        <v>0.34799999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <f>F3*E3</f>
+        <v>0.28200000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
-        <v>0.48</v>
+        <v>3.1E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <f>F4*E4</f>
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>4.7E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
-        <v>0.28200000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <f>F5*E5</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="1">
-        <v>3.1E-2</v>
+        <v>0.39</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="0"/>
-        <v>6.2E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <f>F6*E6</f>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <f>F7*E7</f>
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2">
+        <v>39281023</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" s="1">
-        <v>0.39</v>
+        <v>0.83</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <f>F8*E8</f>
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <f>F9*E9</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" ref="G10:G18" si="0">F10*E10</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="F10" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G14" s="4">
         <f t="shared" si="0"/>
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2">
-        <v>39281023</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="F11" s="1">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5.15</v>
+      </c>
+      <c r="F15">
         <v>1</v>
       </c>
-      <c r="G11" s="1">
-        <f>F11*E11</f>
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" ref="G12:G16" si="1">F12*E12</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1.28</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="F14" s="5">
-        <v>4</v>
-      </c>
-      <c r="G14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="5">
-        <v>0.62</v>
+      <c r="E16" s="4">
+        <v>0.15</v>
       </c>
       <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0.5</v>
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>0.45</v>
       </c>
       <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="5">
-        <v>6.2</v>
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>0.46</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="5">
-        <v>5.15</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21">
-        <v>0.45</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22">
-        <v>0.46</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
     </row>
@@ -1061,18 +959,15 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8"/>
-    <hyperlink ref="D11" r:id="rId9"/>
-    <hyperlink ref="D12" r:id="rId10"/>
-    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed pin headers to smaller ones for lower insertion force.
</commit_message>
<xml_diff>
--- a/communications_hub/Teensy_CommBus_BOM.xlsx
+++ b/communications_hub/Teensy_CommBus_BOM.xlsx
@@ -133,16 +133,16 @@
     <t xml:space="preserve">https://www.digikey.ca/product-detail/en/sunled/XZMYK55W-3/1497-1196-1-ND/4745902</t>
   </si>
   <si>
-    <t xml:space="preserve">CONN RCPT .100" 40POS DUAL TIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSQ-120-03-T-D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN RCPT .100" 30POS DUAL TIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSQ-115-03-T-D</t>
+    <t xml:space="preserve">CONN RCPT 20POS 0.1 GOLD PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSQ-110-03-F-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN RCPT 8POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSQ-104-03-T-D</t>
   </si>
   <si>
     <t xml:space="preserve">RES SMD 62 OHM 1% 1/4W 1206</t>
@@ -524,19 +524,19 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.9081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.0969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,7 +804,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
         <v>37</v>
@@ -816,17 +816,17 @@
         <v>36</v>
       </c>
       <c r="E13" s="10" t="n">
-        <v>6.2</v>
+        <v>3.9</v>
       </c>
       <c r="F13" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13*E13</f>
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
       <c r="B14" s="7" t="s">
         <v>39</v>
@@ -838,14 +838,14 @@
         <v>36</v>
       </c>
       <c r="E14" s="10" t="n">
-        <v>5.15</v>
+        <v>1.16</v>
       </c>
       <c r="F14" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14*E14</f>
-        <v>5.15</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,7 +988,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="17" t="n">
         <f aca="false">SUM(G2:G19)</f>
-        <v>23.916</v>
+        <v>17.626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>